<commit_message>
visualized chlorophyll, sulfate, and pheo data
</commit_message>
<xml_diff>
--- a/Assay Experiment/Round1_assay_sulfate_data.xlsx
+++ b/Assay Experiment/Round1_assay_sulfate_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c9f30cf11edfc58c/virginia tech/research/sulfur methods/AssayData/Round 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c9f30cf11edfc58c/2023 Rtudio/Reservoirs_sulfate/Assay Experiment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="8_{F11D555E-D919-4B61-AB1E-2561B0A8B23C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AFF61FD-3FE9-4867-991D-DBDFD35584D3}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="8_{F11D555E-D919-4B61-AB1E-2561B0A8B23C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02DF0B1D-133F-49FB-8C3B-61064481F2EF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1853" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1852" uniqueCount="163">
   <si>
     <t>Anion Summary Report</t>
   </si>
@@ -519,13 +519,10 @@
     <t>Date</t>
   </si>
   <si>
-    <t>stock</t>
-  </si>
-  <si>
     <t>accidentally spiked</t>
   </si>
   <si>
-    <t>Rep</t>
+    <t>sulfate_stock</t>
   </si>
 </sst>
 </file>
@@ -4962,6 +4959,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5225,20 +5226,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDF79B75-9ED3-461B-AB3B-6B685EC2DFDE}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="126" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="186" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="5" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -5249,16 +5250,13 @@
         <v>159</v>
       </c>
       <c r="D1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E1" t="s">
         <v>160</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -5268,406 +5266,607 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2" s="146">
+      <c r="D2" s="146">
         <v>45838</v>
       </c>
-      <c r="F2" s="21">
+      <c r="E2" s="21">
         <v>844.86633560065991</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>108</v>
       </c>
-      <c r="E3" s="146">
+      <c r="B3">
+        <v>26</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3" s="146">
         <v>45838</v>
       </c>
-      <c r="F3" s="21">
+      <c r="E3" s="21">
         <v>5870.4714437136336</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>109</v>
       </c>
-      <c r="E4" s="146">
+      <c r="B4">
+        <v>35</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4" s="146">
         <v>45838</v>
       </c>
-      <c r="F4" s="21">
+      <c r="E4" s="21">
         <v>7965.9401613815598</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>110</v>
       </c>
-      <c r="E5" s="146">
+      <c r="B5">
+        <v>24</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" s="146">
         <v>45838</v>
       </c>
-      <c r="F5" s="21">
+      <c r="E5" s="21">
         <v>3988.2139014653039</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>111</v>
       </c>
-      <c r="E6" s="146">
+      <c r="B6">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="146">
         <v>45838</v>
       </c>
-      <c r="F6" s="21">
+      <c r="E6" s="21">
         <v>1881.7313930020725</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>112</v>
       </c>
-      <c r="E7" s="146">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" s="146">
         <v>45838</v>
       </c>
-      <c r="F7" s="21">
+      <c r="E7" s="21">
         <v>843.85884332974445</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>113</v>
       </c>
-      <c r="E8" s="146">
+      <c r="B8">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="146">
         <v>45838</v>
       </c>
-      <c r="F8" s="21">
+      <c r="E8" s="21">
         <v>1827.3890172248919</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>114</v>
       </c>
-      <c r="E9" s="146">
+      <c r="B9">
+        <v>24</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9" s="146">
         <v>45838</v>
       </c>
-      <c r="F9" s="21">
+      <c r="E9" s="21">
         <v>5901.909691020036</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>115</v>
       </c>
-      <c r="E10" s="146">
+      <c r="B10">
+        <v>28</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10" s="146">
         <v>45838</v>
       </c>
-      <c r="F10" s="21">
+      <c r="E10" s="21">
         <v>6152.0065219018725</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>116</v>
       </c>
-      <c r="E11" s="146">
+      <c r="B11">
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11" s="146">
         <v>45838</v>
       </c>
-      <c r="F11" s="21">
+      <c r="E11" s="21">
         <v>3973.6404000169405</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>119</v>
       </c>
-      <c r="E12" s="146">
+      <c r="B12">
+        <v>27</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12" s="146">
         <v>45838</v>
       </c>
-      <c r="F12" s="21">
+      <c r="E12" s="21">
         <v>5568.0786072639403</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>120</v>
       </c>
-      <c r="E13" s="146">
+      <c r="B13">
+        <v>19</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13" s="146">
         <v>45838</v>
       </c>
-      <c r="F13" s="21">
+      <c r="E13" s="21">
         <v>4031.6478588476407</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>121</v>
       </c>
-      <c r="E14" s="146">
+      <c r="B14">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="146">
         <v>45838</v>
       </c>
-      <c r="F14" s="21">
+      <c r="E14" s="21">
         <v>1428.6972033303393</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>122</v>
       </c>
-      <c r="E15" s="146">
+      <c r="B15">
+        <v>36</v>
+      </c>
+      <c r="C15">
+        <v>7</v>
+      </c>
+      <c r="D15" s="146">
         <v>45838</v>
       </c>
-      <c r="F15" s="21">
+      <c r="E15" s="21">
         <v>8141.7744665885366</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>123</v>
       </c>
-      <c r="E16" s="146">
+      <c r="B16">
+        <v>23</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16" s="146">
         <v>45838</v>
       </c>
-      <c r="F16" s="21">
+      <c r="E16" s="21">
         <v>3889.4929904142909</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>124</v>
       </c>
-      <c r="E17" s="146">
+      <c r="B17">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="146">
         <v>45838</v>
       </c>
-      <c r="F17" s="21">
+      <c r="E17" s="21">
         <v>1380.9877417222001</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>125</v>
       </c>
-      <c r="E18" s="146">
+      <c r="B18">
+        <v>25</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18" s="146">
         <v>45838</v>
       </c>
-      <c r="F18" s="21">
+      <c r="E18" s="21">
         <v>5912.7913393672861</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>126</v>
       </c>
-      <c r="E19" s="146">
+      <c r="B19">
+        <v>14</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" s="146">
         <v>45838</v>
       </c>
-      <c r="F19" s="21">
+      <c r="E19" s="21">
         <v>1908.2803551406639</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>127</v>
       </c>
-      <c r="E20" s="146">
+      <c r="B20">
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <v>0.5</v>
+      </c>
+      <c r="D20" s="146">
         <v>45838</v>
       </c>
-      <c r="F20" s="21">
+      <c r="E20" s="21">
         <v>1364.1579930857804</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>128</v>
       </c>
-      <c r="E21" s="146">
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" s="146">
         <v>45838</v>
       </c>
-      <c r="F21" s="21">
+      <c r="E21" s="21">
         <v>831.21826319323748</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>131</v>
       </c>
-      <c r="E22" s="146">
+      <c r="B22">
+        <v>31</v>
+      </c>
+      <c r="C22">
+        <v>7</v>
+      </c>
+      <c r="D22" s="146">
         <v>45838</v>
       </c>
-      <c r="F22" s="21">
+      <c r="E22" s="21">
         <v>8527.2895254688301</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>132</v>
       </c>
-      <c r="E23" s="146">
+      <c r="B23">
+        <v>33</v>
+      </c>
+      <c r="C23">
+        <v>7</v>
+      </c>
+      <c r="D23" s="146">
         <v>45838</v>
       </c>
-      <c r="F23" s="21">
+      <c r="E23" s="21">
         <v>7643.4369818322812</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>133</v>
       </c>
-      <c r="E24" s="146">
+      <c r="B24">
+        <v>34</v>
+      </c>
+      <c r="C24">
+        <v>7</v>
+      </c>
+      <c r="D24" s="146">
         <v>45838</v>
       </c>
-      <c r="F24" s="21">
+      <c r="E24" s="21">
         <v>7739.6396315791935</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>134</v>
       </c>
-      <c r="E25" s="146">
+      <c r="B25">
+        <v>16</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" s="146">
         <v>45838</v>
       </c>
-      <c r="F25" s="21">
+      <c r="E25" s="21">
         <v>1853.741275971008</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>135</v>
       </c>
-      <c r="E26" s="146">
+      <c r="B26">
+        <v>30</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+      <c r="D26" s="146">
         <v>45838</v>
       </c>
-      <c r="F26" s="21">
+      <c r="E26" s="21">
         <v>5974.2817057003786</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>136</v>
       </c>
-      <c r="E27" s="146">
+      <c r="B27">
+        <v>22</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27" s="146">
         <v>45838</v>
       </c>
-      <c r="F27" s="21">
+      <c r="E27" s="21">
         <v>3928.2610688415666</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>137</v>
       </c>
-      <c r="E28" s="146">
+      <c r="B28">
+        <v>7</v>
+      </c>
+      <c r="C28">
+        <v>0.5</v>
+      </c>
+      <c r="D28" s="146">
         <v>45838</v>
       </c>
-      <c r="F28" s="21" t="s">
-        <v>162</v>
+      <c r="E28" s="21" t="s">
+        <v>161</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>138</v>
       </c>
-      <c r="E29" s="146">
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29" s="146">
         <v>45838</v>
       </c>
-      <c r="F29" s="21">
+      <c r="E29" s="21">
         <v>869.40469922202692</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>139</v>
       </c>
-      <c r="E30" s="146">
+      <c r="B30">
+        <v>11</v>
+      </c>
+      <c r="C30">
+        <v>0.5</v>
+      </c>
+      <c r="D30" s="146">
         <v>45838</v>
       </c>
-      <c r="F30" s="21">
+      <c r="E30" s="21">
         <v>1390.1507122276071</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>140</v>
       </c>
-      <c r="E31" s="146">
+      <c r="B31">
+        <v>15</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" s="146">
         <v>45838</v>
       </c>
-      <c r="F31" s="21">
+      <c r="E31" s="21">
         <v>1889.8119151074729</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>143</v>
       </c>
-      <c r="E32" s="146">
+      <c r="B32">
+        <v>6</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32" s="146">
         <v>45838</v>
       </c>
-      <c r="F32" s="21">
+      <c r="E32" s="21">
         <v>846.48990378592703</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>144</v>
       </c>
-      <c r="E33" s="146">
+      <c r="B33">
+        <v>13</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33" s="146">
         <v>45838</v>
       </c>
-      <c r="F33" s="21">
+      <c r="E33" s="21">
         <v>1895.512259493396</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>145</v>
       </c>
-      <c r="E34" s="146">
+      <c r="B34">
+        <v>12</v>
+      </c>
+      <c r="C34">
+        <v>0.5</v>
+      </c>
+      <c r="D34" s="146">
         <v>45838</v>
       </c>
-      <c r="F34" s="21">
+      <c r="E34" s="21">
         <v>1368.6517157468786</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>146</v>
       </c>
-      <c r="E35" s="146">
+      <c r="B35">
+        <v>20</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35" s="146">
         <v>45838</v>
       </c>
-      <c r="F35" s="21">
+      <c r="E35" s="21">
         <v>3940.0419391117798</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>147</v>
       </c>
-      <c r="E36" s="146">
+      <c r="B36">
+        <v>32</v>
+      </c>
+      <c r="C36">
+        <v>7</v>
+      </c>
+      <c r="D36" s="146">
         <v>45838</v>
       </c>
-      <c r="F36" s="21">
+      <c r="E36" s="21">
         <v>8661.0458690160394</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>150</v>
       </c>
-      <c r="D37" t="s">
-        <v>161</v>
-      </c>
-      <c r="E37" s="146">
+      <c r="B37" t="s">
+        <v>162</v>
+      </c>
+      <c r="D37" s="146">
         <v>45838</v>
       </c>
-      <c r="F37">
+      <c r="E37">
         <v>1117687</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A14:F44">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A14:E44">
     <sortCondition ref="A14:A44"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>